<commit_message>
* moved histograms to image folder * corrected histograms of impeller scenes * finished test scenes section except raycasted images
</commit_message>
<xml_diff>
--- a/latex/spreadsheets/hq2_hist.xlsx
+++ b/latex/spreadsheets/hq2_hist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="2250" windowWidth="28800" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="hq2_hist" sheetId="1" r:id="rId1"/>
@@ -615,10 +615,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>hq2_hist!$A$2:$A$2564</c:f>
+              <c:f>hq2_hist!$A$2:$A$2565</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2563"/>
+                <c:ptCount val="2564"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -8307,16 +8307,19 @@
                 </c:pt>
                 <c:pt idx="2562">
                   <c:v>2562</c:v>
+                </c:pt>
+                <c:pt idx="2563">
+                  <c:v>2563</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>hq2_hist!$B$2:$B$2564</c:f>
+              <c:f>hq2_hist!$B$2:$B$2565</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2563"/>
+                <c:ptCount val="2564"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -16005,6 +16008,9 @@
                 </c:pt>
                 <c:pt idx="2562">
                   <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2563">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16019,11 +16025,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="453438744"/>
-        <c:axId val="453439136"/>
+        <c:axId val="416529048"/>
+        <c:axId val="537220504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="453438744"/>
+        <c:axId val="416529048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -16080,7 +16086,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453439136"/>
+        <c:crossAx val="537220504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -16090,7 +16096,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="453439136"/>
+        <c:axId val="537220504"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -16148,7 +16154,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="453438744"/>
+        <c:crossAx val="416529048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17046,10 +17052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2564"/>
+  <dimension ref="A1:C2565"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q10" sqref="Q10"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37573,6 +37579,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2565" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2565">
+        <v>2563</v>
+      </c>
+      <c r="B2565">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>